<commit_message>
Refactor BPMN agent initialization, system prompt customization. Updated BPMNTools, improved error handling, and added a new system prompt text area for user customization. Updated requirements to include new dependencies and modified output file path for analysis results.
</commit_message>
<xml_diff>
--- a/data/raw/archives/Error Models/BPMN_Error_Tasks_and_Fixes.xlsx
+++ b/data/raw/archives/Error Models/BPMN_Error_Tasks_and_Fixes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Modelowanie biznesowe\Error Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Modelowanie biznesowe\LLM-BPMN-Checker\data\raw\archives\Error Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62029F7-DE5B-4807-9FA6-60135DA56A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E09425E-AF8C-49D9-B430-CC9317B5CF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors issues identification" sheetId="2" r:id="rId1"/>
@@ -708,11 +708,8 @@
   </sheetPr>
   <dimension ref="A1:W952"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>